<commit_message>
Removed date conversion in ClaimProcessMarine
</commit_message>
<xml_diff>
--- a/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimMapping.xlsx
+++ b/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimMapping.xlsx
@@ -166,9 +166,6 @@
     <t>CauseofLoss</t>
   </si>
   <si>
-    <t>Casue Of Loss</t>
-  </si>
-  <si>
     <t>Basedatafile means, the excel where tool update the latest generated claim number.</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>eBaoClass</t>
   </si>
   <si>
-    <t>eBao</t>
-  </si>
-  <si>
     <t>D/RI</t>
   </si>
   <si>
@@ -197,6 +191,12 @@
   </si>
   <si>
     <t>Recovery From T.P.</t>
+  </si>
+  <si>
+    <t>Cause Of Loss</t>
+  </si>
+  <si>
+    <t>eBao Class</t>
   </si>
 </sst>
 </file>
@@ -534,7 +534,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,29 +765,29 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -827,7 +827,7 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -838,7 +838,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -854,10 +854,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added subrogation expense and cause of loss
</commit_message>
<xml_diff>
--- a/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimMapping.xlsx
+++ b/bin/Debug/netcoreapp3.1/RequiredFiles/ClaimMapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>Key</t>
   </si>
@@ -197,6 +197,27 @@
   </si>
   <si>
     <t>eBao Class</t>
+  </si>
+  <si>
+    <t>VesselPolicyNumber</t>
+  </si>
+  <si>
+    <t>VesselClaimNumber</t>
+  </si>
+  <si>
+    <t>VesselName</t>
+  </si>
+  <si>
+    <t>From VesselRiskinfo excel</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>claim</t>
+  </si>
+  <si>
+    <t>Vessel Name</t>
   </si>
 </sst>
 </file>
@@ -531,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,6 +809,39 @@
       </c>
       <c r="C19" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>